<commit_message>
IGUI 2 fixed create scoop and create mix in flavor logic
</commit_message>
<xml_diff>
--- a/P07/Scrum_MICE_Sprint_2.xlsx
+++ b/P07/Scrum_MICE_Sprint_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rishabh/Desktop/cse1325/P07/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C1A642-3C47-D849-A0DC-97D66F2D9793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466ACED3-F9AF-DA44-8240-45EE7C33EBBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="21600" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="199">
   <si>
     <t>Product Name:</t>
   </si>
@@ -633,6 +633,12 @@
   </si>
   <si>
     <t>Add icons to toolbar and add action listeners and call respective functions</t>
+  </si>
+  <si>
+    <t>Fixed logic to ensure that if not all details are set in create scoop or create mix in flavor, the object won't be added to emporium</t>
+  </si>
+  <si>
+    <t>Completed Day 5</t>
   </si>
 </sst>
 </file>
@@ -2009,19 +2015,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
@@ -7858,7 +7864,7 @@
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -7963,7 +7969,7 @@
       </c>
       <c r="B7" s="18">
         <f>COUNTA(D17:D995)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
@@ -7978,7 +7984,7 @@
       </c>
       <c r="B8" s="18">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -7996,7 +8002,7 @@
       </c>
       <c r="B9" s="18">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -8014,7 +8020,7 @@
       </c>
       <c r="B10" s="18">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -8032,7 +8038,7 @@
       </c>
       <c r="B11" s="18">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -8054,7 +8060,7 @@
       </c>
       <c r="C12" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
@@ -8149,9 +8155,18 @@
       <c r="A18">
         <v>2</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="28"/>
+      <c r="B18" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" t="s">
+        <v>184</v>
+      </c>
+      <c r="D18" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19">

</xml_diff>

<commit_message>
TOOLB 1 completed toolbar and tested
</commit_message>
<xml_diff>
--- a/P07/Scrum_MICE_Sprint_2.xlsx
+++ b/P07/Scrum_MICE_Sprint_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rishabh/Desktop/cse1325/P07/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466ACED3-F9AF-DA44-8240-45EE7C33EBBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F7DE7A-55B4-0C44-ABFA-E5757F47E95F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="21600" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="200">
   <si>
     <t>Product Name:</t>
   </si>
@@ -639,6 +639,9 @@
   </si>
   <si>
     <t>Completed Day 5</t>
+  </si>
+  <si>
+    <t>Finished in Sprint 3</t>
   </si>
 </sst>
 </file>
@@ -1093,7 +1096,7 @@
                   <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>34</c:v>
@@ -2030,13 +2033,13 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3761,7 +3764,7 @@
   <dimension ref="A1:AMJ102"/>
   <sheetViews>
     <sheetView topLeftCell="A11" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -3995,11 +3998,11 @@
       </c>
       <c r="B14" s="4">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C14" s="8">
         <f>COUNTIF(G$24:G$108,"Finished in Sprint 2")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="4"/>
@@ -4023,7 +4026,7 @@
       </c>
       <c r="C15" s="8">
         <f>COUNTIF(G$24:G$108,"Finished in Sprint 3")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="4"/>
@@ -4369,7 +4372,7 @@
         <v>2</v>
       </c>
       <c r="G29" s="14" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
       <c r="H29" s="12" t="s">
         <v>31</v>
@@ -7864,7 +7867,7 @@
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -8056,11 +8059,11 @@
       </c>
       <c r="B12" s="18">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
@@ -8074,7 +8077,7 @@
       </c>
       <c r="B13" s="18">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -8092,7 +8095,7 @@
       </c>
       <c r="B14" s="18">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -8148,7 +8151,7 @@
         <v>196</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="18" spans="1:5">

</xml_diff>

<commit_message>
SAVD LALL SALL in work
</commit_message>
<xml_diff>
--- a/P07/Scrum_MICE_Sprint_2.xlsx
+++ b/P07/Scrum_MICE_Sprint_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rishabh/Desktop/cse1325/P07/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F7DE7A-55B4-0C44-ABFA-E5757F47E95F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20369E20-CBA1-E54A-8BC0-19221028BA56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="21600" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="21600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="200">
   <si>
     <t>Product Name:</t>
   </si>
@@ -1099,16 +1099,16 @@
                   <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>34</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>34</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>34</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>34</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3763,8 +3763,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ102"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32:G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -4022,11 +4022,11 @@
       </c>
       <c r="B15" s="4">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" s="8">
         <f>COUNTIF(G$24:G$108,"Finished in Sprint 3")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="4"/>
@@ -4046,7 +4046,7 @@
       </c>
       <c r="B16" s="4">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="8">
         <f>COUNTIF(G$24:G$108,"Finished in Sprint 4")</f>
@@ -4066,7 +4066,7 @@
       </c>
       <c r="B17" s="4">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17" s="8">
         <f>COUNTIF(G$24:G$108,"Finished in Sprint 5")</f>
@@ -4086,7 +4086,7 @@
       </c>
       <c r="B18" s="4">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" s="8">
         <f>COUNTIF(G$24:G$108,"Finished in Sprint 6")</f>
@@ -4436,7 +4436,7 @@
         <v>3</v>
       </c>
       <c r="G31" s="14" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="H31" s="12" t="s">
         <v>31</v>
@@ -4468,7 +4468,9 @@
       <c r="F32" s="14">
         <v>3</v>
       </c>
-      <c r="G32" s="14"/>
+      <c r="G32" s="14" t="s">
+        <v>195</v>
+      </c>
       <c r="H32" s="12" t="s">
         <v>31</v>
       </c>
@@ -4497,7 +4499,9 @@
       <c r="F33" s="14">
         <v>3</v>
       </c>
-      <c r="G33" s="14"/>
+      <c r="G33" s="14" t="s">
+        <v>195</v>
+      </c>
       <c r="H33" s="12" t="s">
         <v>64</v>
       </c>
@@ -4526,7 +4530,9 @@
       <c r="F34" s="14">
         <v>3</v>
       </c>
-      <c r="G34" s="14"/>
+      <c r="G34" s="14" t="s">
+        <v>195</v>
+      </c>
       <c r="H34" s="12" t="s">
         <v>64</v>
       </c>
@@ -7866,8 +7872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -8175,25 +8181,46 @@
       <c r="A19">
         <v>3</v>
       </c>
-      <c r="B19" s="26"/>
+      <c r="B19" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" t="s">
+        <v>184</v>
+      </c>
       <c r="D19" s="26"/>
-      <c r="E19" s="28"/>
+      <c r="E19" s="28" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20">
         <v>4</v>
       </c>
-      <c r="B20" s="26"/>
+      <c r="B20" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" t="s">
+        <v>184</v>
+      </c>
       <c r="D20" s="26"/>
-      <c r="E20" s="28"/>
+      <c r="E20" s="28" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21">
         <v>5</v>
       </c>
-      <c r="B21" s="26"/>
+      <c r="B21" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" t="s">
+        <v>184</v>
+      </c>
       <c r="D21" s="26"/>
-      <c r="E21" s="28"/>
+      <c r="E21" s="28" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22">
@@ -8872,7 +8899,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>B17:B100</xm:sqref>
+          <xm:sqref>B17:B18 B22:B100</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
SAVD LALL SALL completed and tested
</commit_message>
<xml_diff>
--- a/P07/Scrum_MICE_Sprint_2.xlsx
+++ b/P07/Scrum_MICE_Sprint_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rishabh/Desktop/cse1325/P07/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20369E20-CBA1-E54A-8BC0-19221028BA56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B348B26-C0CA-1B49-8E68-DD498E897CE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="21600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="21600" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="202">
   <si>
     <t>Product Name:</t>
   </si>
@@ -629,9 +629,6 @@
     <t>Slowly draw stylized logo with vectors in About dialog</t>
   </si>
   <si>
-    <t>In Work</t>
-  </si>
-  <si>
     <t>Add icons to toolbar and add action listeners and call respective functions</t>
   </si>
   <si>
@@ -642,6 +639,15 @@
   </si>
   <si>
     <t>Finished in Sprint 3</t>
+  </si>
+  <si>
+    <t>Default file is untitled.mice</t>
+  </si>
+  <si>
+    <t>Load data from speicified file tested and complete</t>
+  </si>
+  <si>
+    <t>Save data works and tested</t>
   </si>
 </sst>
 </file>
@@ -1099,16 +1105,16 @@
                   <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>33</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2018,22 +2024,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -3763,8 +3769,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32:G34"/>
+    <sheetView topLeftCell="A11" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -4022,11 +4028,11 @@
       </c>
       <c r="B15" s="4">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C15" s="8">
         <f>COUNTIF(G$24:G$108,"Finished in Sprint 3")</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="4"/>
@@ -4046,7 +4052,7 @@
       </c>
       <c r="B16" s="4">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C16" s="8">
         <f>COUNTIF(G$24:G$108,"Finished in Sprint 4")</f>
@@ -4066,7 +4072,7 @@
       </c>
       <c r="B17" s="4">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C17" s="8">
         <f>COUNTIF(G$24:G$108,"Finished in Sprint 5")</f>
@@ -4086,7 +4092,7 @@
       </c>
       <c r="B18" s="4">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C18" s="8">
         <f>COUNTIF(G$24:G$108,"Finished in Sprint 6")</f>
@@ -4372,7 +4378,7 @@
         <v>2</v>
       </c>
       <c r="G29" s="14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H29" s="12" t="s">
         <v>31</v>
@@ -4436,7 +4442,7 @@
         <v>3</v>
       </c>
       <c r="G31" s="14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H31" s="12" t="s">
         <v>31</v>
@@ -4469,7 +4475,7 @@
         <v>3</v>
       </c>
       <c r="G32" s="14" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="H32" s="12" t="s">
         <v>31</v>
@@ -4500,7 +4506,7 @@
         <v>3</v>
       </c>
       <c r="G33" s="14" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="H33" s="12" t="s">
         <v>64</v>
@@ -4531,7 +4537,7 @@
         <v>3</v>
       </c>
       <c r="G34" s="14" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="H34" s="12" t="s">
         <v>64</v>
@@ -7872,8 +7878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -7978,7 +7984,7 @@
       </c>
       <c r="B7" s="18">
         <f>COUNTA(D17:D995)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
@@ -7993,7 +7999,7 @@
       </c>
       <c r="B8" s="18">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C8" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -8011,7 +8017,7 @@
       </c>
       <c r="B9" s="18">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C9" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -8029,7 +8035,7 @@
       </c>
       <c r="B10" s="18">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C10" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -8047,7 +8053,7 @@
       </c>
       <c r="B11" s="18">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C11" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -8065,7 +8071,7 @@
       </c>
       <c r="B12" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C12" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -8087,7 +8093,7 @@
       </c>
       <c r="C13" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D13" s="18"/>
       <c r="E13" s="18"/>
@@ -8154,10 +8160,10 @@
         <v>184</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -8171,10 +8177,10 @@
         <v>184</v>
       </c>
       <c r="D18" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="E18" s="28" t="s">
         <v>197</v>
-      </c>
-      <c r="E18" s="28" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -8187,9 +8193,11 @@
       <c r="C19" t="s">
         <v>184</v>
       </c>
-      <c r="D19" s="26"/>
+      <c r="D19" s="26" t="s">
+        <v>199</v>
+      </c>
       <c r="E19" s="28" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -8202,9 +8210,11 @@
       <c r="C20" t="s">
         <v>184</v>
       </c>
-      <c r="D20" s="26"/>
+      <c r="D20" s="26" t="s">
+        <v>200</v>
+      </c>
       <c r="E20" s="28" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -8217,9 +8227,11 @@
       <c r="C21" t="s">
         <v>184</v>
       </c>
-      <c r="D21" s="26"/>
+      <c r="D21" s="26" t="s">
+        <v>201</v>
+      </c>
       <c r="E21" s="28" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="22" spans="1:5">

</xml_diff>

<commit_message>
LOGO added logo with Canvas
</commit_message>
<xml_diff>
--- a/P07/Scrum_MICE_Sprint_2.xlsx
+++ b/P07/Scrum_MICE_Sprint_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rishabh/Desktop/cse1325/P07/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B348B26-C0CA-1B49-8E68-DD498E897CE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A00BEA0C-3954-E044-9E29-D3DAE8D0E6A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="21600" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="21600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="204">
   <si>
     <t>Product Name:</t>
   </si>
@@ -648,6 +648,12 @@
   </si>
   <si>
     <t>Save data works and tested</t>
+  </si>
+  <si>
+    <t>Added logo with Canvas</t>
+  </si>
+  <si>
+    <t>Completed Day 7</t>
   </si>
 </sst>
 </file>
@@ -1105,16 +1111,16 @@
                   <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2024,25 +2030,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -3769,8 +3775,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ102"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -4028,11 +4034,11 @@
       </c>
       <c r="B15" s="4">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="8">
         <f>COUNTIF(G$24:G$108,"Finished in Sprint 3")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="4"/>
@@ -4052,7 +4058,7 @@
       </c>
       <c r="B16" s="4">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" s="8">
         <f>COUNTIF(G$24:G$108,"Finished in Sprint 4")</f>
@@ -4072,7 +4078,7 @@
       </c>
       <c r="B17" s="4">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="8">
         <f>COUNTIF(G$24:G$108,"Finished in Sprint 5")</f>
@@ -4092,7 +4098,7 @@
       </c>
       <c r="B18" s="4">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" s="8">
         <f>COUNTIF(G$24:G$108,"Finished in Sprint 6")</f>
@@ -4410,7 +4416,9 @@
       <c r="F30" s="14">
         <v>3</v>
       </c>
-      <c r="G30" s="14"/>
+      <c r="G30" s="14" t="s">
+        <v>198</v>
+      </c>
       <c r="H30" s="12" t="s">
         <v>54</v>
       </c>
@@ -7878,8 +7886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -7984,7 +7992,7 @@
       </c>
       <c r="B7" s="18">
         <f>COUNTA(D17:D995)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
@@ -7999,7 +8007,7 @@
       </c>
       <c r="B8" s="18">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -8017,7 +8025,7 @@
       </c>
       <c r="B9" s="18">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C9" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -8035,7 +8043,7 @@
       </c>
       <c r="B10" s="18">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C10" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -8053,7 +8061,7 @@
       </c>
       <c r="B11" s="18">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C11" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -8071,7 +8079,7 @@
       </c>
       <c r="B12" s="18">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C12" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -8089,7 +8097,7 @@
       </c>
       <c r="B13" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -8111,7 +8119,7 @@
       </c>
       <c r="C14" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="18"/>
       <c r="E14" s="18"/>
@@ -8238,9 +8246,18 @@
       <c r="A22">
         <v>6</v>
       </c>
-      <c r="B22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="28"/>
+      <c r="B22" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" t="s">
+        <v>184</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="E22" s="28" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23">

</xml_diff>